<commit_message>
Update IP - EX 34 - Atingir metas (Anexo).xlsx
Aplicando uma forma automatica para média
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 34 - Atingir metas (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 34 - Atingir metas (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224C9746-1329-4CAF-9B04-9C7D3B4EB05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96F516D-3C87-485A-962A-88CD28941E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>P1</t>
   </si>
@@ -128,16 +128,26 @@
   </si>
   <si>
     <t>Atingir Metas</t>
+  </si>
+  <si>
+    <t>Média da escola</t>
+  </si>
+  <si>
+    <t>De maneira Automática</t>
+  </si>
+  <si>
+    <t>Nota nessária</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +262,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF22409A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -279,7 +313,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -492,12 +526,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -601,6 +661,24 @@
     </xf>
     <xf numFmtId="44" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1267,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,14 +1528,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:Q16"/>
+  <dimension ref="B1:Q28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1629,7 +1708,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="23">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G14" s="19" t="s">
         <v>28</v>
@@ -1643,7 +1722,9 @@
       <c r="B15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="23">
+        <v>6</v>
+      </c>
       <c r="G15" s="19" t="s">
         <v>27</v>
       </c>
@@ -1658,12 +1739,105 @@
       </c>
       <c r="C16" s="16">
         <f>IFERROR(AVERAGE(C10:C15),"")</f>
-        <v>4</v>
+        <v>4.833333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="49"/>
+    </row>
+    <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="23"/>
+    </row>
+    <row r="26" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B26" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="47">
+        <f>IFERROR(AVERAGE(C20:C25),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B27" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="51">
+        <f>IF(IF(COUNT(C20:C25)=6,
+"Todas as notas inseridas",
+(C27*6-SUM(C20:C25))/(6-COUNT(C20:C25)))&lt;0,0,IF(COUNT(C20:C25)=6,
+"Todas as notas inseridas",
+(C27*6-SUM(C20:C25))/(6-COUNT(C20:C25))))</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <scenarios current="0" show="0" sqref="C16">
+    <scenario name="Média" locked="1" count="6" user="Lorenzo Bianchi" comment="Criado por Lorenzo Bianchi em 06/03/2025_x000a_Alterado por Lorenzo Bianchi em 06/03/2025">
+      <inputCells r="C10" val="3"/>
+      <inputCells r="C11" val="3"/>
+      <inputCells r="C12" val="5"/>
+      <inputCells r="C13" val="7"/>
+      <inputCells r="C14" val="5"/>
+      <inputCells r="C15" val="6"/>
+    </scenario>
+  </scenarios>
+  <mergeCells count="2">
     <mergeCell ref="B2:Q6"/>
+    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>